<commit_message>
napisao sam bla bla
</commit_message>
<xml_diff>
--- a/PIMS-Produkcija 25-04-2019.xlsx
+++ b/PIMS-Produkcija 25-04-2019.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Valentino\Desktop\PIMS-1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2FCA88C-4FBB-4D64-ABEB-848A33085743}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4FDFCD17-A4EA-4399-8F00-940832C48229}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1044" yWindow="2244" windowWidth="17280" windowHeight="8964" xr2:uid="{CDD3BD0B-B75A-4F90-8A25-5C1F1036C15F}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{CDD3BD0B-B75A-4F90-8A25-5C1F1036C15F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -128,9 +128,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="668" uniqueCount="232">
   <si>
-    <t>RN</t>
-  </si>
-  <si>
     <t>Opis</t>
   </si>
   <si>
@@ -1168,6 +1165,9 @@
   </si>
   <si>
     <t>Reklamacijski proces- postavke i upute</t>
+  </si>
+  <si>
+    <t>blalba</t>
   </si>
 </sst>
 </file>
@@ -2074,7 +2074,7 @@
       <pane xSplit="2" ySplit="1" topLeftCell="C16" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="H16" sqref="H16"/>
+      <selection pane="bottomRight"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" outlineLevelCol="1" x14ac:dyDescent="0.3"/>
@@ -2103,60 +2103,60 @@
   <sheetData>
     <row r="1" spans="1:21" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A1" s="39" t="s">
+        <v>231</v>
+      </c>
+      <c r="B1" s="39" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="39" t="s">
+      <c r="C1" s="39" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="39" t="s">
+      <c r="D1" s="39" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="39" t="s">
+      <c r="E1" s="39" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="39" t="s">
+      <c r="F1" s="39" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="39" t="s">
+      <c r="G1" s="39" t="s">
         <v>5</v>
-      </c>
-      <c r="G1" s="39" t="s">
-        <v>6</v>
       </c>
       <c r="H1" s="39"/>
       <c r="I1" s="39"/>
       <c r="J1" s="39" t="s">
+        <v>6</v>
+      </c>
+      <c r="K1" s="39" t="s">
         <v>7</v>
       </c>
-      <c r="K1" s="39" t="s">
+      <c r="L1" s="39" t="s">
         <v>8</v>
       </c>
-      <c r="L1" s="39" t="s">
+      <c r="M1" s="33" t="s">
         <v>9</v>
       </c>
-      <c r="M1" s="33" t="s">
+      <c r="N1" s="47" t="s">
+        <v>210</v>
+      </c>
+      <c r="O1" s="47" t="s">
+        <v>212</v>
+      </c>
+      <c r="P1" s="47" t="s">
         <v>10</v>
       </c>
-      <c r="N1" s="47" t="s">
-        <v>211</v>
-      </c>
-      <c r="O1" s="47" t="s">
-        <v>213</v>
-      </c>
-      <c r="P1" s="47" t="s">
+      <c r="Q1" s="47" t="s">
         <v>11</v>
       </c>
-      <c r="Q1" s="47" t="s">
+      <c r="R1" s="47" t="s">
         <v>12</v>
       </c>
-      <c r="R1" s="47" t="s">
+      <c r="S1" s="85" t="s">
         <v>13</v>
       </c>
-      <c r="S1" s="85" t="s">
+      <c r="T1" s="46" t="s">
         <v>14</v>
-      </c>
-      <c r="T1" s="46" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="2" spans="1:21" ht="58.2" thickBot="1" x14ac:dyDescent="0.35">
@@ -2164,16 +2164,16 @@
         <v>77870</v>
       </c>
       <c r="B2" s="50" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C2" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D2" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="D2" s="3" t="s">
-        <v>18</v>
-      </c>
       <c r="E2" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F2" s="4">
         <v>43488.48333333333</v>
@@ -2189,10 +2189,10 @@
         <v>0.25</v>
       </c>
       <c r="J2" s="36" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="K2" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="L2" s="8">
         <v>43496</v>
@@ -2206,16 +2206,16 @@
         <v>Ante</v>
       </c>
       <c r="P2" s="24" t="s">
+        <v>25</v>
+      </c>
+      <c r="Q2" s="64" t="s">
         <v>26</v>
       </c>
-      <c r="Q2" s="64" t="s">
-        <v>27</v>
-      </c>
       <c r="R2" s="24" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="S2" s="65" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="T2" s="61"/>
       <c r="U2" s="2"/>
@@ -2225,16 +2225,16 @@
         <v>77867</v>
       </c>
       <c r="B3" s="50" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C3" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D3" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="D3" s="3" t="s">
-        <v>18</v>
-      </c>
       <c r="E3" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F3" s="4">
         <v>43488.453472222223</v>
@@ -2250,10 +2250,10 @@
         <v>0.33333333333333331</v>
       </c>
       <c r="J3" s="36" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="K3" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="L3" s="8">
         <v>43496</v>
@@ -2267,16 +2267,16 @@
         <v>Ante</v>
       </c>
       <c r="P3" s="24" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="Q3" s="28" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="R3" s="24" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="S3" s="57" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
     </row>
     <row r="4" spans="1:21" s="2" customFormat="1" ht="54" hidden="1" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -2284,16 +2284,16 @@
         <v>77868</v>
       </c>
       <c r="B4" s="50" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C4" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D4" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="D4" s="3" t="s">
-        <v>18</v>
-      </c>
       <c r="E4" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F4" s="4">
         <v>43488.463194444441</v>
@@ -2309,10 +2309,10 @@
         <v>0.16666666666666666</v>
       </c>
       <c r="J4" s="36" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="K4" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="L4" s="8">
         <v>43496</v>
@@ -2326,16 +2326,16 @@
         <v>Ante</v>
       </c>
       <c r="P4" s="24" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="Q4" s="28" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="R4" s="24" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="S4" s="57" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
     <row r="5" spans="1:21" s="2" customFormat="1" ht="15" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -2343,16 +2343,16 @@
         <v>63144</v>
       </c>
       <c r="B5" s="50" t="s">
+        <v>22</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="E5" s="3" t="s">
         <v>23</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="D5" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="E5" s="3" t="s">
-        <v>24</v>
       </c>
       <c r="F5" s="4">
         <v>42881.381249999999</v>
@@ -2368,10 +2368,10 @@
         <v>79.3</v>
       </c>
       <c r="J5" s="36" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="K5" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="L5" s="8">
         <v>43496</v>
@@ -2385,14 +2385,14 @@
         <v>Ante</v>
       </c>
       <c r="P5" s="24" t="s">
+        <v>25</v>
+      </c>
+      <c r="Q5" s="28" t="s">
         <v>26</v>
-      </c>
-      <c r="Q5" s="28" t="s">
-        <v>27</v>
       </c>
       <c r="R5" s="24"/>
       <c r="S5" s="58" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="6" spans="1:21" s="2" customFormat="1" ht="15" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -2400,13 +2400,13 @@
         <v>63144</v>
       </c>
       <c r="B6" s="50" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C6" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D6" s="3" t="s">
         <v>17</v>
-      </c>
-      <c r="D6" s="3" t="s">
-        <v>18</v>
       </c>
       <c r="E6" s="3"/>
       <c r="F6" s="4">
@@ -2423,10 +2423,10 @@
         <v>7.416666666666667</v>
       </c>
       <c r="J6" s="36" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="K6" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="L6" s="8">
         <v>43496</v>
@@ -2440,14 +2440,14 @@
         <v>Ante</v>
       </c>
       <c r="P6" s="24" t="s">
+        <v>25</v>
+      </c>
+      <c r="Q6" s="28" t="s">
         <v>26</v>
-      </c>
-      <c r="Q6" s="28" t="s">
-        <v>27</v>
       </c>
       <c r="R6" s="24"/>
       <c r="S6" s="58" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="7" spans="1:21" s="2" customFormat="1" ht="43.8" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -2455,17 +2455,17 @@
         <v>77578</v>
       </c>
       <c r="B7" s="50" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E7" s="3"/>
       <c r="F7" s="3" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="G7" s="5">
         <v>0</v>
@@ -2478,10 +2478,10 @@
         <v>0.66666666666666663</v>
       </c>
       <c r="J7" s="10" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="K7" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="L7" s="8">
         <v>43495</v>
@@ -2495,14 +2495,14 @@
         <v>Marijana</v>
       </c>
       <c r="P7" s="24" t="s">
+        <v>110</v>
+      </c>
+      <c r="Q7" s="28" t="s">
         <v>111</v>
-      </c>
-      <c r="Q7" s="28" t="s">
-        <v>112</v>
       </c>
       <c r="R7" s="28"/>
       <c r="S7" s="58" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="8" spans="1:21" s="2" customFormat="1" ht="58.2" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -2510,13 +2510,13 @@
         <v>77659</v>
       </c>
       <c r="B8" s="50" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E8" s="3"/>
       <c r="F8" s="4">
@@ -2533,10 +2533,10 @@
         <v>0.16666666666666666</v>
       </c>
       <c r="J8" s="10" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="K8" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="L8" s="8">
         <v>43504</v>
@@ -2550,14 +2550,14 @@
         <v>Marijana</v>
       </c>
       <c r="P8" s="24" t="s">
+        <v>110</v>
+      </c>
+      <c r="Q8" s="28" t="s">
         <v>111</v>
-      </c>
-      <c r="Q8" s="28" t="s">
-        <v>112</v>
       </c>
       <c r="R8" s="28"/>
       <c r="S8" s="58" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="9" spans="1:21" s="2" customFormat="1" ht="58.2" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -2565,13 +2565,13 @@
         <v>77375</v>
       </c>
       <c r="B9" s="50" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="E9" s="3"/>
       <c r="F9" s="38">
@@ -2588,10 +2588,10 @@
         <v>0.33333333333333331</v>
       </c>
       <c r="J9" s="10" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="K9" s="3" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="L9" s="8">
         <v>43480</v>
@@ -2605,20 +2605,20 @@
         <v>Zvonimir</v>
       </c>
       <c r="P9" s="24" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="Q9" s="28" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="R9" s="24"/>
       <c r="S9" s="57" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="T9" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="U9" s="2" t="s">
         <v>128</v>
-      </c>
-      <c r="U9" s="2" t="s">
-        <v>129</v>
       </c>
     </row>
     <row r="10" spans="1:21" s="2" customFormat="1" ht="43.8" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -2626,16 +2626,16 @@
         <v>74766</v>
       </c>
       <c r="B10" s="50" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C10" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="D10" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="D10" s="3" t="s">
-        <v>18</v>
-      </c>
       <c r="E10" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F10" s="4">
         <v>43374.662499999999</v>
@@ -2651,10 +2651,10 @@
         <v>1.8333333333333335</v>
       </c>
       <c r="J10" s="10" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="K10" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="L10" s="8">
         <v>43511</v>
@@ -2670,14 +2670,14 @@
         <v>Ante</v>
       </c>
       <c r="P10" s="24" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="Q10" s="28" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="R10" s="28"/>
       <c r="S10" s="58" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="11" spans="1:21" s="2" customFormat="1" ht="29.4" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -2685,16 +2685,16 @@
         <v>77435</v>
       </c>
       <c r="B11" s="50" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C11" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D11" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="D11" s="3" t="s">
-        <v>18</v>
-      </c>
       <c r="E11" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F11" s="12">
         <v>43475.469444444447</v>
@@ -2710,16 +2710,16 @@
         <v>1.8333333333333335</v>
       </c>
       <c r="J11" s="10" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="K11" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="L11" s="8">
         <v>43483</v>
       </c>
       <c r="M11" s="34" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="N11" s="41">
         <v>43511</v>
@@ -2729,17 +2729,17 @@
         <v>Ante</v>
       </c>
       <c r="P11" s="26" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="Q11" s="28" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="R11" s="28"/>
       <c r="S11" s="59" t="s">
+        <v>61</v>
+      </c>
+      <c r="T11" s="2" t="s">
         <v>62</v>
-      </c>
-      <c r="T11" s="2" t="s">
-        <v>63</v>
       </c>
     </row>
     <row r="12" spans="1:21" s="2" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
@@ -2747,16 +2747,16 @@
         <v>72481</v>
       </c>
       <c r="B12" s="50" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C12" s="15" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F12" s="4">
         <v>43262.606249999997</v>
@@ -2772,10 +2772,10 @@
         <v>2.3333333333333335</v>
       </c>
       <c r="J12" s="10" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="K12" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="L12" s="8">
         <v>43503</v>
@@ -2789,14 +2789,14 @@
         <v>Zagi</v>
       </c>
       <c r="P12" s="28" t="s">
+        <v>43</v>
+      </c>
+      <c r="Q12" s="28" t="s">
         <v>44</v>
-      </c>
-      <c r="Q12" s="28" t="s">
-        <v>45</v>
       </c>
       <c r="R12" s="28"/>
       <c r="S12" s="85" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="U12" s="8">
         <v>43518</v>
@@ -2807,16 +2807,16 @@
         <v>75320</v>
       </c>
       <c r="B13" s="50" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C13" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="D13" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="D13" s="3" t="s">
-        <v>18</v>
-      </c>
       <c r="E13" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F13" s="4">
         <v>43395.688194444447</v>
@@ -2832,10 +2832,10 @@
         <v>1</v>
       </c>
       <c r="J13" s="10" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="K13" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="L13" s="8">
         <v>43518</v>
@@ -2851,14 +2851,14 @@
         <v>Ante</v>
       </c>
       <c r="P13" s="24" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="Q13" s="28" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="R13" s="28"/>
       <c r="S13" s="57" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="14" spans="1:21" s="2" customFormat="1" ht="126" customHeight="1" x14ac:dyDescent="0.3">
@@ -2866,13 +2866,13 @@
         <v>72480</v>
       </c>
       <c r="B14" s="50" t="s">
+        <v>41</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D14" s="3" t="s">
         <v>42</v>
-      </c>
-      <c r="C14" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="D14" s="3" t="s">
-        <v>43</v>
       </c>
       <c r="E14" s="3"/>
       <c r="F14" s="4">
@@ -2889,10 +2889,10 @@
         <v>6.25</v>
       </c>
       <c r="J14" s="10" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="K14" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="L14" s="8">
         <v>43525</v>
@@ -2906,14 +2906,14 @@
         <v>Zagi</v>
       </c>
       <c r="P14" s="28" t="s">
+        <v>43</v>
+      </c>
+      <c r="Q14" s="28" t="s">
         <v>44</v>
-      </c>
-      <c r="Q14" s="28" t="s">
-        <v>45</v>
       </c>
       <c r="R14" s="28"/>
       <c r="S14" s="85" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="U14" s="8">
         <v>43525</v>
@@ -2924,13 +2924,13 @@
         <v>73537</v>
       </c>
       <c r="B15" s="50" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E15" s="3"/>
       <c r="F15" s="38">
@@ -2947,10 +2947,10 @@
         <v>0.83333333333333337</v>
       </c>
       <c r="J15" s="10" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="K15" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="L15" s="8">
         <v>43502</v>
@@ -2964,14 +2964,14 @@
         <v>Marijana</v>
       </c>
       <c r="P15" s="24" t="s">
+        <v>56</v>
+      </c>
+      <c r="Q15" s="28" t="s">
         <v>57</v>
-      </c>
-      <c r="Q15" s="28" t="s">
-        <v>58</v>
       </c>
       <c r="R15" s="28"/>
       <c r="S15" s="57" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="16" spans="1:21" s="2" customFormat="1" ht="26.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -2979,13 +2979,13 @@
         <v>72549</v>
       </c>
       <c r="B16" s="51" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E16" s="3"/>
       <c r="F16" s="4">
@@ -3002,10 +3002,10 @@
         <v>2</v>
       </c>
       <c r="J16" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="K16" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="L16" s="8"/>
       <c r="M16" s="8"/>
@@ -3017,16 +3017,16 @@
         <v>Marijana</v>
       </c>
       <c r="P16" s="28" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="Q16" s="28" t="s">
+        <v>47</v>
+      </c>
+      <c r="R16" s="28" t="s">
         <v>48</v>
       </c>
-      <c r="R16" s="28" t="s">
+      <c r="S16" s="85" t="s">
         <v>49</v>
-      </c>
-      <c r="S16" s="85" t="s">
-        <v>50</v>
       </c>
       <c r="U16" s="8">
         <v>43560</v>
@@ -3037,16 +3037,16 @@
         <v>75191</v>
       </c>
       <c r="B17" s="50" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C17" s="15" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E17" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F17" s="4">
         <v>43390.445138888892</v>
@@ -3062,10 +3062,10 @@
         <v>10</v>
       </c>
       <c r="J17" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="K17" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="L17" s="44">
         <v>43536</v>
@@ -3079,14 +3079,14 @@
         <v>Zagi</v>
       </c>
       <c r="P17" s="28" t="s">
+        <v>43</v>
+      </c>
+      <c r="Q17" s="28" t="s">
         <v>44</v>
-      </c>
-      <c r="Q17" s="28" t="s">
-        <v>45</v>
       </c>
       <c r="R17" s="28"/>
       <c r="S17" s="85" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="U17" s="8">
         <v>43504</v>
@@ -3097,16 +3097,16 @@
         <v>75194</v>
       </c>
       <c r="B18" s="50" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C18" s="15" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E18" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F18" s="4">
         <v>43390.454861111109</v>
@@ -3122,10 +3122,10 @@
         <v>5</v>
       </c>
       <c r="J18" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="K18" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="L18" s="44">
         <v>43536</v>
@@ -3139,14 +3139,14 @@
         <v>Zagi</v>
       </c>
       <c r="P18" s="29" t="s">
+        <v>43</v>
+      </c>
+      <c r="Q18" s="28" t="s">
         <v>44</v>
-      </c>
-      <c r="Q18" s="28" t="s">
-        <v>45</v>
       </c>
       <c r="R18" s="28"/>
       <c r="S18" s="85" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="U18" s="8">
         <v>43497</v>
@@ -3157,13 +3157,13 @@
         <v>75822</v>
       </c>
       <c r="B19" s="53" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E19" s="3"/>
       <c r="F19" s="4">
@@ -3180,10 +3180,10 @@
         <v>1.25</v>
       </c>
       <c r="J19" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="K19" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="L19" s="8">
         <v>43504</v>
@@ -3197,16 +3197,16 @@
         <v>Marijana</v>
       </c>
       <c r="P19" s="63" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="Q19" s="64" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="R19" s="63" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="S19" s="86" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="20" spans="1:21" s="2" customFormat="1" ht="29.4" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -3214,16 +3214,16 @@
         <v>77677</v>
       </c>
       <c r="B20" s="50" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E20" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F20" s="4">
         <v>43482.352777777778</v>
@@ -3239,10 +3239,10 @@
         <v>0.83333333333333337</v>
       </c>
       <c r="J20" s="10" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="K20" s="3" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="L20" s="8">
         <v>43490</v>
@@ -3256,14 +3256,14 @@
         <v>Joe</v>
       </c>
       <c r="P20" s="28" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="Q20" s="28" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="R20" s="28"/>
       <c r="S20" s="58" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="21" spans="1:21" s="2" customFormat="1" ht="53.25" customHeight="1" x14ac:dyDescent="0.3">
@@ -3271,13 +3271,13 @@
         <v>77613</v>
       </c>
       <c r="B21" s="53" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D21" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E21" s="3"/>
       <c r="F21" s="4">
@@ -3294,10 +3294,10 @@
         <v>0.33333333333333331</v>
       </c>
       <c r="J21" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="K21" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="L21" s="8">
         <v>43524</v>
@@ -3311,16 +3311,16 @@
         <v>Marijana</v>
       </c>
       <c r="P21" s="28" t="s">
+        <v>132</v>
+      </c>
+      <c r="Q21" s="28" t="s">
         <v>133</v>
       </c>
-      <c r="Q21" s="28" t="s">
-        <v>134</v>
-      </c>
       <c r="R21" s="24" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="S21" s="85" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="22" spans="1:21" s="2" customFormat="1" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
@@ -3328,19 +3328,19 @@
         <v>79226</v>
       </c>
       <c r="B22" s="50" t="s">
+        <v>173</v>
+      </c>
+      <c r="C22" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D22" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="E22" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="F22" s="38" t="s">
         <v>174</v>
-      </c>
-      <c r="C22" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="D22" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="E22" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="F22" s="38" t="s">
-        <v>175</v>
       </c>
       <c r="G22" s="39">
         <v>1</v>
@@ -3353,10 +3353,10 @@
         <v>1.5</v>
       </c>
       <c r="J22" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="K22" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="L22" s="8"/>
       <c r="N22" s="27">
@@ -3367,14 +3367,14 @@
         <v>Zagi</v>
       </c>
       <c r="P22" s="28" t="s">
+        <v>43</v>
+      </c>
+      <c r="Q22" s="28" t="s">
         <v>44</v>
-      </c>
-      <c r="Q22" s="28" t="s">
-        <v>45</v>
       </c>
       <c r="R22" s="28"/>
       <c r="S22" s="85" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
     </row>
     <row r="23" spans="1:21" s="2" customFormat="1" ht="43.8" thickTop="1" x14ac:dyDescent="0.3">
@@ -3382,19 +3382,19 @@
         <v>79228</v>
       </c>
       <c r="B23" s="50" t="s">
+        <v>175</v>
+      </c>
+      <c r="C23" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D23" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="E23" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="F23" s="38" t="s">
         <v>176</v>
-      </c>
-      <c r="C23" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="D23" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="E23" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="F23" s="38" t="s">
-        <v>177</v>
       </c>
       <c r="G23" s="39">
         <v>2</v>
@@ -3407,10 +3407,10 @@
         <v>2.1666666666666665</v>
       </c>
       <c r="J23" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="K23" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="L23" s="8"/>
       <c r="N23" s="27">
@@ -3421,14 +3421,14 @@
         <v>Zagi</v>
       </c>
       <c r="P23" s="28" t="s">
+        <v>43</v>
+      </c>
+      <c r="Q23" s="28" t="s">
         <v>44</v>
-      </c>
-      <c r="Q23" s="28" t="s">
-        <v>45</v>
       </c>
       <c r="R23" s="28"/>
       <c r="S23" s="85" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
     <row r="24" spans="1:21" s="2" customFormat="1" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
@@ -3436,13 +3436,13 @@
         <v>75197</v>
       </c>
       <c r="B24" s="53" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D24" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E24" s="3"/>
       <c r="F24" s="4">
@@ -3459,10 +3459,10 @@
         <v>0.16666666666666666</v>
       </c>
       <c r="J24" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="K24" s="3" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="L24" s="44">
         <v>43543</v>
@@ -3476,16 +3476,16 @@
         <v>Zagi</v>
       </c>
       <c r="P24" s="63" t="s">
+        <v>43</v>
+      </c>
+      <c r="Q24" s="64" t="s">
         <v>44</v>
       </c>
-      <c r="Q24" s="64" t="s">
-        <v>45</v>
-      </c>
       <c r="R24" s="64" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="S24" s="86" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
     </row>
     <row r="25" spans="1:21" s="2" customFormat="1" ht="133.19999999999999" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -3493,13 +3493,13 @@
         <v>77672</v>
       </c>
       <c r="B25" s="53" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D25" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E25" s="3"/>
       <c r="F25" s="4">
@@ -3516,10 +3516,10 @@
         <v>3.5</v>
       </c>
       <c r="J25" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="K25" s="3" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="L25" s="8">
         <v>43496</v>
@@ -3533,16 +3533,16 @@
         <v>Marijana</v>
       </c>
       <c r="P25" s="24" t="s">
+        <v>110</v>
+      </c>
+      <c r="Q25" s="28" t="s">
         <v>111</v>
       </c>
-      <c r="Q25" s="28" t="s">
-        <v>112</v>
-      </c>
       <c r="R25" s="28" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="S25" s="85" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="26" spans="1:21" s="2" customFormat="1" ht="44.4" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -3550,16 +3550,16 @@
         <v>78314</v>
       </c>
       <c r="B26" s="50" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D26" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E26" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F26" s="38">
         <v>43510.604166666664</v>
@@ -3573,10 +3573,10 @@
         <v>1</v>
       </c>
       <c r="J26" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="K26" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="L26" s="8">
         <v>43524</v>
@@ -3589,10 +3589,10 @@
         <v>Zagi</v>
       </c>
       <c r="P26" s="28" t="s">
+        <v>43</v>
+      </c>
+      <c r="Q26" s="28" t="s">
         <v>44</v>
-      </c>
-      <c r="Q26" s="28" t="s">
-        <v>45</v>
       </c>
       <c r="R26" s="28"/>
       <c r="S26" s="85"/>
@@ -3602,19 +3602,19 @@
         <v>79236</v>
       </c>
       <c r="B27" s="50" t="s">
+        <v>177</v>
+      </c>
+      <c r="C27" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D27" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="E27" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="F27" s="38" t="s">
         <v>178</v>
-      </c>
-      <c r="C27" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="D27" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="E27" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="F27" s="38" t="s">
-        <v>179</v>
       </c>
       <c r="G27" s="39">
         <v>0</v>
@@ -3627,10 +3627,10 @@
         <v>0.33333333333333331</v>
       </c>
       <c r="J27" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="K27" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="L27" s="8"/>
       <c r="N27" s="27">
@@ -3641,14 +3641,14 @@
         <v>Zagi</v>
       </c>
       <c r="P27" s="64" t="s">
+        <v>43</v>
+      </c>
+      <c r="Q27" s="64" t="s">
         <v>44</v>
-      </c>
-      <c r="Q27" s="64" t="s">
-        <v>45</v>
       </c>
       <c r="R27" s="64"/>
       <c r="S27" s="86" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
     </row>
     <row r="28" spans="1:21" s="2" customFormat="1" ht="409.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -3656,7 +3656,7 @@
         <v>79473</v>
       </c>
       <c r="B28" s="56" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="C28" s="16"/>
       <c r="D28" s="3"/>
@@ -3673,19 +3673,19 @@
         <v>43546</v>
       </c>
       <c r="O28" s="79" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="P28" s="63" t="s">
+        <v>110</v>
+      </c>
+      <c r="Q28" s="64" t="s">
         <v>111</v>
       </c>
-      <c r="Q28" s="64" t="s">
-        <v>112</v>
-      </c>
       <c r="R28" s="24" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="S28" s="86" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
     </row>
     <row r="29" spans="1:21" s="2" customFormat="1" ht="44.4" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -3693,16 +3693,16 @@
         <v>76355</v>
       </c>
       <c r="B29" s="50" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C29" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="D29" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="D29" s="3" t="s">
-        <v>18</v>
-      </c>
       <c r="E29" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F29" s="4">
         <v>43433.654166666667</v>
@@ -3718,10 +3718,10 @@
         <v>0.66666666666666663</v>
       </c>
       <c r="J29" s="36" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="K29" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="L29" s="8">
         <v>43497</v>
@@ -3737,16 +3737,16 @@
         <v>Ante</v>
       </c>
       <c r="P29" s="24" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="Q29" s="28" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="R29" s="28" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="S29" s="57" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
     </row>
     <row r="30" spans="1:21" s="2" customFormat="1" ht="102" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -3754,16 +3754,16 @@
         <v>77864</v>
       </c>
       <c r="B30" s="50" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C30" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D30" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="D30" s="3" t="s">
-        <v>18</v>
-      </c>
       <c r="E30" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F30" s="4">
         <v>43488.447916666664</v>
@@ -3779,10 +3779,10 @@
         <v>0.33333333333333331</v>
       </c>
       <c r="J30" s="36" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="K30" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="L30" s="8">
         <v>43496</v>
@@ -3796,16 +3796,16 @@
         <v>Ante</v>
       </c>
       <c r="P30" s="24" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="Q30" s="28" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="R30" s="24" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="S30" s="57" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="31" spans="1:21" s="2" customFormat="1" ht="87.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -3813,16 +3813,16 @@
         <v>71460</v>
       </c>
       <c r="B31" s="50" t="s">
+        <v>37</v>
+      </c>
+      <c r="C31" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D31" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="E31" s="3" t="s">
         <v>38</v>
-      </c>
-      <c r="C31" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="D31" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="E31" s="3" t="s">
-        <v>39</v>
       </c>
       <c r="F31" s="4">
         <v>43221.572916666664</v>
@@ -3838,16 +3838,16 @@
         <v>26.583333333333332</v>
       </c>
       <c r="J31" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="K31" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="L31" s="8">
         <v>43511</v>
       </c>
       <c r="M31" s="49" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="N31" s="25">
         <v>43553</v>
@@ -3857,19 +3857,19 @@
         <v>Ante</v>
       </c>
       <c r="P31" s="26" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q31" s="28" t="s">
         <v>31</v>
       </c>
-      <c r="Q31" s="28" t="s">
-        <v>32</v>
-      </c>
       <c r="R31" s="28" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="S31" s="68" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="T31" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="32" spans="1:21" s="2" customFormat="1" ht="73.2" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -3877,16 +3877,16 @@
         <v>75670</v>
       </c>
       <c r="B32" s="50" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C32" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="D32" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="D32" s="3" t="s">
-        <v>18</v>
-      </c>
       <c r="E32" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F32" s="4">
         <v>43411.59097222222</v>
@@ -3902,10 +3902,10 @@
         <v>1.0833333333333333</v>
       </c>
       <c r="J32" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="K32" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="L32" s="8">
         <v>43518</v>
@@ -3921,16 +3921,16 @@
         <v>Ante</v>
       </c>
       <c r="P32" s="24" t="s">
+        <v>43</v>
+      </c>
+      <c r="Q32" s="28" t="s">
         <v>44</v>
       </c>
-      <c r="Q32" s="28" t="s">
-        <v>45</v>
-      </c>
       <c r="R32" s="28" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="S32" s="57" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="33" spans="1:21" s="2" customFormat="1" ht="231.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -3938,13 +3938,13 @@
         <v>76356</v>
       </c>
       <c r="B33" s="50" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C33" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D33" s="3" t="s">
         <v>17</v>
-      </c>
-      <c r="D33" s="3" t="s">
-        <v>18</v>
       </c>
       <c r="E33" s="3"/>
       <c r="F33" s="4">
@@ -3961,10 +3961,10 @@
         <v>0.58333333333333337</v>
       </c>
       <c r="J33" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="K33" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="L33" s="8">
         <v>43518</v>
@@ -3980,16 +3980,16 @@
         <v>Ante</v>
       </c>
       <c r="P33" s="24" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="Q33" s="28" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="R33" s="28" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="S33" s="57" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
     </row>
     <row r="34" spans="1:21" s="2" customFormat="1" ht="44.4" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -3997,16 +3997,16 @@
         <v>75280</v>
       </c>
       <c r="B34" s="51" t="s">
+        <v>74</v>
+      </c>
+      <c r="C34" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D34" s="3" t="s">
         <v>75</v>
       </c>
-      <c r="C34" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="D34" s="3" t="s">
-        <v>76</v>
-      </c>
       <c r="E34" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F34" s="38">
         <v>43393.368750000001</v>
@@ -4022,10 +4022,10 @@
         <v>3.35</v>
       </c>
       <c r="J34" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="K34" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="L34" s="8">
         <v>43553</v>
@@ -4039,10 +4039,10 @@
         <v>Zvonimir</v>
       </c>
       <c r="P34" s="28" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="Q34" s="28" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="R34" s="28"/>
       <c r="S34" s="57"/>
@@ -4055,13 +4055,13 @@
         <v>76642</v>
       </c>
       <c r="B35" s="55" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C35" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D35" s="3" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="E35" s="3"/>
       <c r="F35" s="38">
@@ -4078,10 +4078,10 @@
         <v>0.51666666666666672</v>
       </c>
       <c r="J35" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="K35" s="3" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="L35" s="8">
         <v>43504</v>
@@ -4097,14 +4097,14 @@
         <v>Zvonimir</v>
       </c>
       <c r="P35" s="24" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="Q35" s="28" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="R35" s="24"/>
       <c r="S35" s="57" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="36" spans="1:21" s="2" customFormat="1" x14ac:dyDescent="0.3">
@@ -4112,16 +4112,16 @@
         <v>77529</v>
       </c>
       <c r="B36" s="55" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C36" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D36" s="3" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="E36" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F36" s="38">
         <v>43479.479166666664</v>
@@ -4137,10 +4137,10 @@
         <v>0.33333333333333331</v>
       </c>
       <c r="J36" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="K36" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="L36" s="8">
         <v>43503</v>
@@ -4156,14 +4156,14 @@
         <v>Zvonimir</v>
       </c>
       <c r="P36" s="24" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="Q36" s="28" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="R36" s="24"/>
       <c r="S36" s="57" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="U36" s="2">
         <v>4</v>
@@ -4174,13 +4174,13 @@
         <v>77683</v>
       </c>
       <c r="B37" s="51" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="C37" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D37" s="3" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="E37" s="3"/>
       <c r="F37" s="38">
@@ -4197,10 +4197,10 @@
         <v>2.0166666666666666</v>
       </c>
       <c r="J37" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="K37" s="3" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="L37" s="8">
         <v>43511</v>
@@ -4214,14 +4214,14 @@
         <v>Zvonimir</v>
       </c>
       <c r="P37" s="63" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="Q37" s="64" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="R37" s="64"/>
       <c r="S37" s="65" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="38" spans="1:21" s="2" customFormat="1" ht="43.8" thickTop="1" x14ac:dyDescent="0.3">
@@ -4229,19 +4229,19 @@
         <v>78316</v>
       </c>
       <c r="B38" s="50" t="s">
+        <v>167</v>
+      </c>
+      <c r="C38" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D38" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="E38" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="F38" s="38" t="s">
         <v>168</v>
-      </c>
-      <c r="C38" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="D38" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="E38" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="F38" s="38" t="s">
-        <v>169</v>
       </c>
       <c r="G38" s="39">
         <v>0</v>
@@ -4254,10 +4254,10 @@
         <v>0.25</v>
       </c>
       <c r="J38" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="K38" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="L38" s="8"/>
       <c r="N38" s="27">
@@ -4268,10 +4268,10 @@
         <v>Zagi</v>
       </c>
       <c r="P38" s="28" t="s">
+        <v>43</v>
+      </c>
+      <c r="Q38" s="28" t="s">
         <v>44</v>
-      </c>
-      <c r="Q38" s="28" t="s">
-        <v>45</v>
       </c>
       <c r="R38" s="28"/>
       <c r="S38" s="85"/>
@@ -4281,13 +4281,13 @@
         <v>75323</v>
       </c>
       <c r="B39" s="51" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C39" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D39" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E39" s="3"/>
       <c r="F39" s="4">
@@ -4304,10 +4304,10 @@
         <v>0.33333333333333331</v>
       </c>
       <c r="J39" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="K39" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="L39" s="8">
         <v>43556</v>
@@ -4317,19 +4317,19 @@
         <v>43556</v>
       </c>
       <c r="O39" s="26" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="P39" s="24" t="s">
+        <v>85</v>
+      </c>
+      <c r="Q39" s="28" t="s">
+        <v>69</v>
+      </c>
+      <c r="R39" s="28" t="s">
+        <v>48</v>
+      </c>
+      <c r="S39" s="85" t="s">
         <v>86</v>
-      </c>
-      <c r="Q39" s="28" t="s">
-        <v>70</v>
-      </c>
-      <c r="R39" s="28" t="s">
-        <v>49</v>
-      </c>
-      <c r="S39" s="85" t="s">
-        <v>87</v>
       </c>
     </row>
     <row r="40" spans="1:21" s="2" customFormat="1" ht="30" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -4337,13 +4337,13 @@
         <v>77622</v>
       </c>
       <c r="B40" s="51" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C40" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D40" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E40" s="3"/>
       <c r="F40" s="4">
@@ -4360,10 +4360,10 @@
         <v>0.16666666666666666</v>
       </c>
       <c r="J40" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="K40" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="L40" s="8">
         <v>43556</v>
@@ -4373,19 +4373,19 @@
         <v>43556</v>
       </c>
       <c r="O40" s="31" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="P40" s="28" t="s">
+        <v>20</v>
+      </c>
+      <c r="Q40" s="28" t="s">
         <v>21</v>
       </c>
-      <c r="Q40" s="28" t="s">
-        <v>22</v>
-      </c>
       <c r="R40" s="28" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="S40" s="87" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="U40" s="8">
         <v>43553</v>
@@ -4396,16 +4396,16 @@
         <v>74349</v>
       </c>
       <c r="B41" s="50" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C41" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="D41" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="D41" s="3" t="s">
-        <v>18</v>
-      </c>
       <c r="E41" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F41" s="4">
         <v>43356.558333333334</v>
@@ -4421,10 +4421,10 @@
         <v>1.6833333333333333</v>
       </c>
       <c r="J41" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="K41" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="L41" s="8">
         <v>43511</v>
@@ -4440,16 +4440,16 @@
         <v>Ante</v>
       </c>
       <c r="P41" s="24" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q41" s="28" t="s">
         <v>31</v>
       </c>
-      <c r="Q41" s="28" t="s">
-        <v>32</v>
-      </c>
       <c r="R41" s="28" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="S41" s="57" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="U41" s="32">
         <v>43549</v>
@@ -4460,16 +4460,16 @@
         <v>75157</v>
       </c>
       <c r="B42" s="50" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C42" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="D42" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="D42" s="3" t="s">
-        <v>18</v>
-      </c>
       <c r="E42" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F42" s="4">
         <v>43389.470138888886</v>
@@ -4485,10 +4485,10 @@
         <v>1.1666666666666667</v>
       </c>
       <c r="J42" s="10" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="K42" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="L42" s="8">
         <v>43511</v>
@@ -4504,16 +4504,16 @@
         <v>Ante</v>
       </c>
       <c r="P42" s="28" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="Q42" s="28" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="R42" s="28" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="S42" s="57" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="43" spans="1:21" s="2" customFormat="1" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
@@ -4521,13 +4521,13 @@
         <v>77063</v>
       </c>
       <c r="B43" s="53" t="s">
+        <v>120</v>
+      </c>
+      <c r="C43" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D43" s="3" t="s">
         <v>121</v>
-      </c>
-      <c r="C43" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="D43" s="3" t="s">
-        <v>122</v>
       </c>
       <c r="E43" s="3"/>
       <c r="F43" s="38">
@@ -4544,10 +4544,10 @@
         <v>0.5</v>
       </c>
       <c r="J43" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="K43" s="3" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="L43" s="8">
         <v>43525</v>
@@ -4561,17 +4561,17 @@
         <v>Filip</v>
       </c>
       <c r="P43" s="28" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="Q43" s="28" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="R43" s="28"/>
       <c r="S43" s="57" t="s">
+        <v>123</v>
+      </c>
+      <c r="T43" s="2" t="s">
         <v>124</v>
-      </c>
-      <c r="T43" s="2" t="s">
-        <v>125</v>
       </c>
       <c r="U43" s="8">
         <v>43539</v>
@@ -4582,13 +4582,13 @@
         <v>77991</v>
       </c>
       <c r="B44" s="52" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="C44" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D44" s="3" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="E44" s="3"/>
       <c r="F44" s="38">
@@ -4603,10 +4603,10 @@
         <v>4</v>
       </c>
       <c r="J44" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="K44" s="3" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="L44" s="8">
         <v>43511</v>
@@ -4620,14 +4620,14 @@
         <v>Filip</v>
       </c>
       <c r="P44" s="24" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="Q44" s="28" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="R44" s="28"/>
       <c r="S44" s="57" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
     <row r="45" spans="1:21" s="2" customFormat="1" ht="58.8" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -4635,16 +4635,16 @@
         <v>77874</v>
       </c>
       <c r="B45" s="51" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C45" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D45" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="D45" s="3" t="s">
-        <v>18</v>
-      </c>
       <c r="E45" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F45" s="4">
         <v>43488.504861111112</v>
@@ -4660,10 +4660,10 @@
         <v>0.66666666666666663</v>
       </c>
       <c r="J45" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="K45" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="L45" s="8">
         <v>43525</v>
@@ -4679,16 +4679,16 @@
         <v>Ante</v>
       </c>
       <c r="P45" s="28" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="Q45" s="28" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="R45" s="28" t="s">
+        <v>199</v>
+      </c>
+      <c r="S45" s="57" t="s">
         <v>200</v>
-      </c>
-      <c r="S45" s="57" t="s">
-        <v>201</v>
       </c>
       <c r="U45" s="8">
         <v>43532</v>
@@ -4699,13 +4699,13 @@
         <v>77871</v>
       </c>
       <c r="B46" s="50" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C46" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D46" s="3" t="s">
         <v>17</v>
-      </c>
-      <c r="D46" s="3" t="s">
-        <v>18</v>
       </c>
       <c r="E46" s="3"/>
       <c r="F46" s="4">
@@ -4722,10 +4722,10 @@
         <v>0.33333333333333331</v>
       </c>
       <c r="J46" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="K46" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="L46" s="8">
         <v>43525</v>
@@ -4741,16 +4741,16 @@
         <v>Ante</v>
       </c>
       <c r="P46" s="24" t="s">
+        <v>150</v>
+      </c>
+      <c r="Q46" s="28" t="s">
         <v>151</v>
       </c>
-      <c r="Q46" s="28" t="s">
-        <v>152</v>
-      </c>
       <c r="R46" s="28" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="S46" s="57" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="47" spans="1:21" s="2" customFormat="1" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -4758,13 +4758,13 @@
         <v>77674</v>
       </c>
       <c r="B47" s="53" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="C47" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D47" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E47" s="3"/>
       <c r="F47" s="4">
@@ -4781,13 +4781,13 @@
         <v>1.8333333333333335</v>
       </c>
       <c r="J47" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="K47" s="3" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="L47" s="45" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="M47" s="8"/>
       <c r="N47" s="27">
@@ -4798,12 +4798,12 @@
         <v>Marijana</v>
       </c>
       <c r="P47" s="28" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="Q47" s="28"/>
       <c r="R47" s="28"/>
       <c r="S47" s="85" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="48" spans="1:21" s="2" customFormat="1" ht="44.4" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -4811,13 +4811,13 @@
         <v>74031</v>
       </c>
       <c r="B48" s="51" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C48" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D48" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E48" s="3"/>
       <c r="F48" s="4">
@@ -4834,10 +4834,10 @@
         <v>0.16666666666666666</v>
       </c>
       <c r="J48" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="K48" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="L48" s="8">
         <v>43581</v>
@@ -4851,7 +4851,7 @@
         <v>Marijana</v>
       </c>
       <c r="P48" s="28" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="Q48" s="28"/>
       <c r="R48" s="28"/>
@@ -4873,19 +4873,19 @@
         <v>43574</v>
       </c>
       <c r="O49" s="26" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="P49" s="24" t="s">
+        <v>25</v>
+      </c>
+      <c r="Q49" s="28" t="s">
         <v>26</v>
       </c>
-      <c r="Q49" s="28" t="s">
-        <v>27</v>
-      </c>
       <c r="R49" s="24" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="S49" s="57" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
     </row>
     <row r="50" spans="1:21" s="2" customFormat="1" ht="30" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -4893,16 +4893,16 @@
         <v>75321</v>
       </c>
       <c r="B50" s="51" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C50" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="D50" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="D50" s="3" t="s">
-        <v>18</v>
-      </c>
       <c r="E50" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F50" s="4">
         <v>43395.703472222223</v>
@@ -4918,10 +4918,10 @@
         <v>2.3333333333333335</v>
       </c>
       <c r="J50" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="K50" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="L50" s="8">
         <v>43518</v>
@@ -4937,13 +4937,13 @@
         <v>Ante</v>
       </c>
       <c r="P50" s="24" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="Q50" s="28" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="R50" s="28" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="S50" s="57"/>
     </row>
@@ -4952,16 +4952,16 @@
         <v>64865</v>
       </c>
       <c r="B51" s="51" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C51" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D51" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="D51" s="3" t="s">
-        <v>18</v>
-      </c>
       <c r="E51" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F51" s="4">
         <v>42972.40625</v>
@@ -4977,16 +4977,16 @@
         <v>1.85</v>
       </c>
       <c r="J51" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="K51" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="L51" s="8">
         <v>43560</v>
       </c>
       <c r="M51" s="37" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="N51" s="25">
         <v>43581</v>
@@ -4996,13 +4996,13 @@
         <v>Ante</v>
       </c>
       <c r="P51" s="28" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q51" s="28" t="s">
         <v>31</v>
       </c>
-      <c r="Q51" s="28" t="s">
-        <v>32</v>
-      </c>
       <c r="R51" s="28" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="S51" s="57"/>
       <c r="U51" s="8">
@@ -5014,16 +5014,16 @@
         <v>77879</v>
       </c>
       <c r="B52" s="51" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C52" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D52" s="3" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="E52" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F52" s="38">
         <v>43488.567361111112</v>
@@ -5039,10 +5039,10 @@
         <v>0.5</v>
       </c>
       <c r="J52" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="K52" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="L52" s="8">
         <v>43581</v>
@@ -5056,14 +5056,14 @@
         <v>Zvonimir</v>
       </c>
       <c r="P52" s="28" t="s">
+        <v>160</v>
+      </c>
+      <c r="Q52" s="28" t="s">
         <v>161</v>
-      </c>
-      <c r="Q52" s="28" t="s">
-        <v>162</v>
       </c>
       <c r="R52" s="28"/>
       <c r="S52" s="92" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="U52" s="8">
         <v>43581</v>
@@ -5074,13 +5074,13 @@
         <v>63775</v>
       </c>
       <c r="B53" s="51" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C53" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D53" s="3" t="s">
         <v>17</v>
-      </c>
-      <c r="D53" s="3" t="s">
-        <v>18</v>
       </c>
       <c r="E53" s="3"/>
       <c r="F53" s="4">
@@ -5097,16 +5097,16 @@
         <v>2</v>
       </c>
       <c r="J53" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="K53" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="L53" s="8">
         <v>43567</v>
       </c>
       <c r="M53" s="37" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="N53" s="25">
         <v>43581</v>
@@ -5116,13 +5116,13 @@
         <v>Ante</v>
       </c>
       <c r="P53" s="28" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="Q53" s="28" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="R53" s="28" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="S53" s="57"/>
       <c r="U53" s="8">
@@ -5147,19 +5147,19 @@
         <v>43581</v>
       </c>
       <c r="O54" s="26" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="P54" s="24" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="Q54" s="28" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="R54" s="28" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="S54" s="57" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
     </row>
     <row r="55" spans="1:21" s="2" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -5167,16 +5167,16 @@
         <v>76643</v>
       </c>
       <c r="B55" s="54" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C55" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D55" s="3" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="E55" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F55" s="38">
         <v>43444.365277777775</v>
@@ -5192,10 +5192,10 @@
         <v>0.41666666666666669</v>
       </c>
       <c r="J55" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="K55" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="L55" s="8">
         <v>43646</v>
@@ -5211,15 +5211,15 @@
         <v>Zvonimir</v>
       </c>
       <c r="P55" s="63" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="Q55" s="64" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="R55" s="63"/>
       <c r="S55" s="65"/>
       <c r="U55" s="2" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="56" spans="1:21" s="2" customFormat="1" ht="30" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
@@ -5227,13 +5227,13 @@
         <v>77572</v>
       </c>
       <c r="B56" s="51" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C56" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D56" s="3" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="E56" s="3"/>
       <c r="F56" s="38">
@@ -5250,10 +5250,10 @@
         <v>0.66666666666666663</v>
       </c>
       <c r="J56" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="K56" s="3" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="L56" s="8">
         <v>43646</v>
@@ -5267,14 +5267,14 @@
         <v>Zvonimir</v>
       </c>
       <c r="P56" s="24" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="Q56" s="28" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="R56" s="24"/>
       <c r="S56" s="93" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="57" spans="1:21" s="2" customFormat="1" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
@@ -5282,16 +5282,16 @@
         <v>74413</v>
       </c>
       <c r="B57" s="50" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C57" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="D57" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="D57" s="3" t="s">
-        <v>18</v>
-      </c>
       <c r="E57" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F57" s="4">
         <v>43361.430555555555</v>
@@ -5307,10 +5307,10 @@
         <v>1</v>
       </c>
       <c r="J57" s="10" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="K57" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="L57" s="8">
         <v>43518</v>
@@ -5319,21 +5319,21 @@
         <v>2.5</v>
       </c>
       <c r="N57" s="42" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="O57" s="80" t="str">
         <f t="shared" si="6"/>
         <v>Ante</v>
       </c>
       <c r="P57" s="28" t="s">
+        <v>43</v>
+      </c>
+      <c r="Q57" s="28" t="s">
         <v>44</v>
-      </c>
-      <c r="Q57" s="28" t="s">
-        <v>45</v>
       </c>
       <c r="R57" s="28"/>
       <c r="S57" s="58" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="U57" s="8">
         <v>43511</v>
@@ -5344,19 +5344,19 @@
         <v>79218</v>
       </c>
       <c r="B58" s="54" t="s">
+        <v>169</v>
+      </c>
+      <c r="C58" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D58" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="E58" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="F58" s="38" t="s">
         <v>170</v>
-      </c>
-      <c r="C58" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="D58" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="E58" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="F58" s="38" t="s">
-        <v>171</v>
       </c>
       <c r="G58" s="39">
         <v>0</v>
@@ -5369,28 +5369,28 @@
         <v>0.16666666666666666</v>
       </c>
       <c r="J58" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="K58" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="L58" s="8"/>
       <c r="N58" s="50" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="O58" s="82" t="str">
         <f t="shared" si="6"/>
         <v>Ante</v>
       </c>
       <c r="P58" s="28" t="s">
+        <v>43</v>
+      </c>
+      <c r="Q58" s="28" t="s">
         <v>44</v>
-      </c>
-      <c r="Q58" s="28" t="s">
-        <v>45</v>
       </c>
       <c r="R58" s="28"/>
       <c r="S58" s="57" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="59" spans="1:21" s="2" customFormat="1" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
@@ -5398,13 +5398,13 @@
         <v>71012</v>
       </c>
       <c r="B59" s="53" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C59" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D59" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E59" s="3"/>
       <c r="F59" s="4">
@@ -5421,33 +5421,33 @@
         <v>4.833333333333333</v>
       </c>
       <c r="J59" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="K59" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="L59" s="45" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="M59" s="45"/>
       <c r="N59" s="67" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="O59" s="26" t="str">
         <f t="shared" si="6"/>
         <v>Marijana</v>
       </c>
       <c r="P59" s="24" t="s">
+        <v>34</v>
+      </c>
+      <c r="Q59" s="28" t="s">
         <v>35</v>
       </c>
-      <c r="Q59" s="28" t="s">
+      <c r="R59" s="24" t="s">
         <v>36</v>
       </c>
-      <c r="R59" s="24" t="s">
-        <v>37</v>
-      </c>
       <c r="S59" s="87" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
     </row>
     <row r="60" spans="1:21" s="2" customFormat="1" ht="15" thickTop="1" x14ac:dyDescent="0.3">
@@ -5455,16 +5455,16 @@
         <v>73389</v>
       </c>
       <c r="B60" s="51" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C60" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D60" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E60" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="F60" s="4">
         <v>43306.447916666664</v>
@@ -5480,10 +5480,10 @@
         <v>0.5</v>
       </c>
       <c r="J60" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="K60" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="L60" s="8">
         <v>43524</v>
@@ -5499,7 +5499,7 @@
       <c r="R60" s="28"/>
       <c r="S60" s="57"/>
       <c r="T60" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="61" spans="1:21" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
@@ -5507,13 +5507,13 @@
         <v>77383</v>
       </c>
       <c r="B61" s="51" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="C61" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D61" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E61" s="3"/>
       <c r="F61" s="4">
@@ -5530,10 +5530,10 @@
         <v>0.5</v>
       </c>
       <c r="J61" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="K61" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="N61" s="43"/>
       <c r="O61" s="83" t="str">
@@ -5541,7 +5541,7 @@
         <v>Marijana</v>
       </c>
       <c r="P61" s="28" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="Q61" s="28"/>
       <c r="R61" s="28"/>
@@ -5552,16 +5552,16 @@
         <v>77094</v>
       </c>
       <c r="B62" s="50" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C62" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D62" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="D62" s="3" t="s">
-        <v>18</v>
-      </c>
       <c r="E62" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="F62" s="4">
         <v>43465.482638888891</v>
@@ -5577,16 +5577,16 @@
         <v>1</v>
       </c>
       <c r="J62" s="10" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="K62" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="L62" s="8">
         <v>43493</v>
       </c>
       <c r="M62" s="34" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="N62" s="41"/>
       <c r="O62" s="77" t="str">
@@ -5594,17 +5594,17 @@
         <v>Ante</v>
       </c>
       <c r="P62" s="26" t="s">
+        <v>43</v>
+      </c>
+      <c r="Q62" s="28" t="s">
         <v>44</v>
-      </c>
-      <c r="Q62" s="28" t="s">
-        <v>45</v>
       </c>
       <c r="R62" s="31"/>
       <c r="S62" s="59" t="s">
+        <v>78</v>
+      </c>
+      <c r="T62" s="2" t="s">
         <v>79</v>
-      </c>
-      <c r="T62" s="2" t="s">
-        <v>80</v>
       </c>
     </row>
     <row r="63" spans="1:21" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
@@ -5612,13 +5612,13 @@
         <v>77885</v>
       </c>
       <c r="B63" s="50" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C63" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D63" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E63" s="3"/>
       <c r="F63" s="4">
@@ -5635,10 +5635,10 @@
         <v>4.5</v>
       </c>
       <c r="J63" s="10" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="K63" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="L63" s="8">
         <v>43497</v>
@@ -5658,13 +5658,13 @@
         <v>73972</v>
       </c>
       <c r="B64" s="50" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C64" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="D64" s="3" t="s">
         <v>17</v>
-      </c>
-      <c r="D64" s="3" t="s">
-        <v>18</v>
       </c>
       <c r="E64" s="3"/>
       <c r="F64" s="4">
@@ -5681,13 +5681,13 @@
         <v>3.3333333333333335</v>
       </c>
       <c r="J64" s="10" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="K64" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="M64" s="34" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="N64" s="43"/>
       <c r="O64" s="83" t="str">
@@ -5698,7 +5698,7 @@
       <c r="Q64" s="28"/>
       <c r="R64" s="28"/>
       <c r="S64" s="58" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="65" spans="1:20" s="2" customFormat="1" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
@@ -5706,16 +5706,16 @@
         <v>74627</v>
       </c>
       <c r="B65" s="50" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C65" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="D65" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="D65" s="3" t="s">
-        <v>18</v>
-      </c>
       <c r="E65" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F65" s="4">
         <v>43368.647222222222</v>
@@ -5731,13 +5731,13 @@
         <v>0.83333333333333337</v>
       </c>
       <c r="J65" s="10" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="K65" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="M65" s="34" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="N65" s="43"/>
       <c r="O65" s="83" t="str">
@@ -5745,15 +5745,15 @@
         <v>Ante</v>
       </c>
       <c r="P65" s="28" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="Q65" s="28"/>
       <c r="R65" s="28"/>
       <c r="S65" s="43" t="s">
+        <v>90</v>
+      </c>
+      <c r="T65" s="2" t="s">
         <v>91</v>
-      </c>
-      <c r="T65" s="2" t="s">
-        <v>92</v>
       </c>
     </row>
     <row r="66" spans="1:20" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
@@ -5761,16 +5761,16 @@
         <v>75680</v>
       </c>
       <c r="B66" s="50" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C66" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="D66" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="D66" s="3" t="s">
-        <v>18</v>
-      </c>
       <c r="E66" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F66" s="4">
         <v>43411.686805555553</v>
@@ -5786,16 +5786,16 @@
         <v>0.83333333333333337</v>
       </c>
       <c r="J66" s="10" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="K66" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="L66" s="8">
         <v>43504</v>
       </c>
       <c r="M66" s="34" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="N66" s="43"/>
       <c r="O66" s="83" t="str">
@@ -5803,14 +5803,14 @@
         <v>Ante</v>
       </c>
       <c r="P66" s="28" t="s">
+        <v>93</v>
+      </c>
+      <c r="Q66" s="28" t="s">
         <v>94</v>
-      </c>
-      <c r="Q66" s="28" t="s">
-        <v>95</v>
       </c>
       <c r="R66" s="28"/>
       <c r="S66" s="58" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="67" spans="1:20" s="2" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
@@ -5818,16 +5818,16 @@
         <v>77876</v>
       </c>
       <c r="B67" s="50" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C67" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D67" s="3" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E67" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F67" s="4">
         <v>43488.526388888888</v>
@@ -5843,10 +5843,10 @@
         <v>0.25</v>
       </c>
       <c r="J67" s="10" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="K67" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="L67" s="8">
         <v>43496</v>
@@ -5860,14 +5860,14 @@
         <v>Joe</v>
       </c>
       <c r="P67" s="28" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="Q67" s="28" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="R67" s="28"/>
       <c r="S67" s="57" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="68" spans="1:20" s="2" customFormat="1" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
@@ -5875,16 +5875,16 @@
         <v>78315</v>
       </c>
       <c r="B68" s="50" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="C68" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D68" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E68" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F68" s="38">
         <v>43510.604166666664</v>
@@ -5898,10 +5898,10 @@
         <v>3</v>
       </c>
       <c r="J68" s="10" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="K68" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="L68" s="8">
         <v>43511</v>
@@ -5912,16 +5912,16 @@
         <v>Zagi</v>
       </c>
       <c r="P68" s="28" t="s">
+        <v>43</v>
+      </c>
+      <c r="Q68" s="28" t="s">
         <v>44</v>
       </c>
-      <c r="Q68" s="28" t="s">
-        <v>45</v>
-      </c>
       <c r="R68" s="28" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="S68" s="94" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="69" spans="1:20" s="2" customFormat="1" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
@@ -5929,13 +5929,13 @@
         <v>77211</v>
       </c>
       <c r="B69" s="50" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C69" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D69" s="3" t="s">
         <v>17</v>
-      </c>
-      <c r="D69" s="3" t="s">
-        <v>18</v>
       </c>
       <c r="E69" s="3"/>
       <c r="F69" s="4">
@@ -5952,13 +5952,13 @@
         <v>21.416666666666668</v>
       </c>
       <c r="J69" s="36" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="K69" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="M69" s="34" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="N69" s="43"/>
       <c r="O69" s="83" t="str">
@@ -5969,7 +5969,7 @@
       <c r="Q69" s="28"/>
       <c r="R69" s="28"/>
       <c r="S69" s="58" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="70" spans="1:20" s="2" customFormat="1" ht="86.4" x14ac:dyDescent="0.3">
@@ -5990,19 +5990,19 @@
         <v>43581</v>
       </c>
       <c r="O70" s="26" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="P70" s="24" t="s">
+        <v>25</v>
+      </c>
+      <c r="Q70" s="28" t="s">
         <v>26</v>
       </c>
-      <c r="Q70" s="28" t="s">
-        <v>27</v>
-      </c>
       <c r="R70" s="24" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="S70" s="57" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
     </row>
     <row r="71" spans="1:20" s="2" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
@@ -6023,19 +6023,19 @@
         <v>43553</v>
       </c>
       <c r="O71" s="26" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="P71" s="24" t="s">
+        <v>110</v>
+      </c>
+      <c r="Q71" s="28" t="s">
         <v>111</v>
       </c>
-      <c r="Q71" s="28" t="s">
-        <v>112</v>
-      </c>
       <c r="R71" s="28" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="S71" s="85" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
     </row>
     <row r="72" spans="1:20" s="2" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
@@ -6056,15 +6056,15 @@
         <v>43553</v>
       </c>
       <c r="O72" s="26" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="P72" s="24"/>
       <c r="Q72" s="28"/>
       <c r="R72" s="28" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="S72" s="85" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="73" spans="1:20" s="2" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
@@ -6072,13 +6072,13 @@
         <v>77875</v>
       </c>
       <c r="B73" s="50" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C73" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D73" s="3" t="s">
         <v>17</v>
-      </c>
-      <c r="D73" s="3" t="s">
-        <v>18</v>
       </c>
       <c r="E73" s="3"/>
       <c r="F73" s="4">
@@ -6095,10 +6095,10 @@
         <v>0.5</v>
       </c>
       <c r="J73" s="10" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="K73" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="L73" s="8">
         <v>43525</v>
@@ -6114,16 +6114,16 @@
         <v>Ante</v>
       </c>
       <c r="P73" s="24" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="Q73" s="28" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="R73" s="28" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="S73" s="57" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="74" spans="1:20" s="2" customFormat="1" ht="90.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -6131,16 +6131,16 @@
         <v>76350</v>
       </c>
       <c r="B74" s="51" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C74" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="D74" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="D74" s="3" t="s">
-        <v>18</v>
-      </c>
       <c r="E74" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F74" s="4">
         <v>43433.602083333331</v>
@@ -6156,16 +6156,16 @@
         <v>1.1000000000000001</v>
       </c>
       <c r="J74" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="K74" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="L74" s="8">
         <v>43525</v>
       </c>
       <c r="M74" s="37" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="N74" s="25">
         <v>43595</v>
@@ -6175,13 +6175,13 @@
         <v>Ante</v>
       </c>
       <c r="P74" s="24" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="Q74" s="28" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="R74" s="28" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="S74" s="57"/>
     </row>
@@ -6190,13 +6190,13 @@
         <v>79925</v>
       </c>
       <c r="B75" s="96" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="C75" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="D75" s="3" t="s">
         <v>17</v>
-      </c>
-      <c r="D75" s="3" t="s">
-        <v>18</v>
       </c>
       <c r="E75" s="3"/>
       <c r="F75" s="97">
@@ -6213,26 +6213,26 @@
         <v>0.5</v>
       </c>
       <c r="J75" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="K75" s="3"/>
       <c r="N75" s="25">
         <v>43593</v>
       </c>
       <c r="O75" s="26" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="P75" s="24" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="Q75" s="28" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="R75" s="24" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="S75" s="85" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="76" spans="1:20" s="2" customFormat="1" x14ac:dyDescent="0.3">
@@ -6292,7 +6292,7 @@
       <c r="Q78" s="48"/>
       <c r="R78" s="21"/>
       <c r="S78" s="88" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="79" spans="1:20" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -6313,17 +6313,17 @@
       <c r="Q79" s="48"/>
       <c r="R79" s="21"/>
       <c r="S79" s="89" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="80" spans="1:20" x14ac:dyDescent="0.3">
       <c r="S80" s="90" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="81" spans="19:19" x14ac:dyDescent="0.3">
       <c r="S81" s="90" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
   </sheetData>
@@ -6428,15 +6428,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101009A1684ECC1F8F94F9020A16343972D0E" ma:contentTypeVersion="2" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="52368caef71303477d5faaa4dae2859e">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="cf73b2c2-8002-4efa-aeba-97f797406057" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="4b1ccb08a93107023b84ab2a3dfdb272" ns2:_="">
     <xsd:import namespace="cf73b2c2-8002-4efa-aeba-97f797406057"/>
@@ -6568,6 +6559,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2C3D0553-B273-4B8B-9C51-9BBA805E503E}">
   <ds:schemaRefs>
@@ -6585,14 +6585,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E9CAC86F-5D5F-48A7-9D12-449BE140A0A3}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E7B0587F-3A52-4D14-8E3A-078EC86DE28C}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -6608,4 +6600,12 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E9CAC86F-5D5F-48A7-9D12-449BE140A0A3}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>